<commit_message>
Research on Keyboard Scanning and Flowchart
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Log Book.xlsx
+++ b/Documentation/Complete Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D6125FF-5802-4EB6-9EF1-9095CE873139}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{040A07B3-2FD2-4089-8413-1C9CF56A1A3C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Read about Keyboard Matrixes and Keypress Ghositng, Forse Sensitive Resistors, Guitar Fret Distance Calculation Algorithms</t>
+  </si>
+  <si>
+    <t>11.10.2022</t>
+  </si>
+  <si>
+    <t>Research Keyboards</t>
+  </si>
+  <si>
+    <t>Research on Keyboard Scanning and Create Flowchart</t>
   </si>
 </sst>
 </file>
@@ -576,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,41 +962,61 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="E19">
+        <v>80</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="3">
-        <f>SUM(E2:E20)</f>
-        <v>1735</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="3">
+        <f>SUM(E2:E21)</f>
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="3">
-        <f>E21 / 60</f>
-        <v>28.916666666666668</v>
+      <c r="E23" s="3">
+        <f>E22 / 60</f>
+        <v>30.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Key Switch Interfaces: Buses, Matrix, Debounce
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Log Book.xlsx
+++ b/Documentation/Complete Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{040A07B3-2FD2-4089-8413-1C9CF56A1A3C}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF296672-A581-4068-BC07-F157C6560DDA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Research on Keyboard Scanning and Create Flowchart</t>
+  </si>
+  <si>
+    <t>Research Key Switch Interface Design: Buses, Matrix, Debouncing</t>
   </si>
 </sst>
 </file>
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,41 +985,61 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="E20">
+        <v>240</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="3">
-        <f>SUM(E2:E21)</f>
-        <v>1815</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="3">
+        <f>SUM(E2:E22)</f>
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="3">
-        <f>E22 / 60</f>
-        <v>30.25</v>
+      <c r="E24" s="3">
+        <f>E23 / 60</f>
+        <v>34.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cost, Target Audience, Marketability and Feasibility
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Log Book.xlsx
+++ b/Documentation/Complete Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{919A37AF-9204-4714-9CDC-0AE5E22BCC3B}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB4B2874-7E4D-45EA-9F0D-0442BB20F012}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -249,6 +249,18 @@
   </si>
   <si>
     <t>User Requirements: Complete</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Constraints Chapter: Scope and Limitations</t>
+  </si>
+  <si>
+    <t>Cost, Marketability, Feasibility</t>
+  </si>
+  <si>
+    <t>Chapters Cost (research prototype parts for estimation), Target Audience, Marketability, Feasibility and Social Aspects for Success</t>
   </si>
 </sst>
 </file>
@@ -630,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,35 +1218,75 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D31" s="2" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29">
+        <v>55</v>
+      </c>
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30">
+        <v>220</v>
+      </c>
+      <c r="F30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="2">
-        <f>SUM(E2:E27)</f>
-        <v>2850</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D32" s="2" t="s">
+      <c r="E39" s="2">
+        <f>SUM(E2:E30)</f>
+        <v>3255</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="2">
-        <f>E31 / 60</f>
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="E40" s="2">
+        <f>E39 / 60</f>
+        <v>54.25</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>37</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D41" t="s">
         <v>40</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E41" t="s">
         <v>36</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F41" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Risk Analysis and Methodologies
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Log Book.xlsx
+++ b/Documentation/Complete Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB4B2874-7E4D-45EA-9F0D-0442BB20F012}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C0E80C7-A9A8-4277-8727-7C6462E9DFEC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -261,6 +261,21 @@
   </si>
   <si>
     <t>Chapters Cost (research prototype parts for estimation), Target Audience, Marketability, Feasibility and Social Aspects for Success</t>
+  </si>
+  <si>
+    <t>17.10.2022</t>
+  </si>
+  <si>
+    <t>Risk Analysis</t>
+  </si>
+  <si>
+    <t>Collect Relevant Risk Factors, Severity, Probability, and Organise it in a Table</t>
+  </si>
+  <si>
+    <t>Methodologies</t>
+  </si>
+  <si>
+    <t>Research Methdologies Suitable for Individual Projects, Document Waterfall, TDD, KanBan, and Justify Chosen Methodologies</t>
   </si>
 </sst>
 </file>
@@ -645,7 +660,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,13 +1273,53 @@
         <v>74</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31">
+        <v>95</v>
+      </c>
+      <c r="F31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32">
+        <v>190</v>
+      </c>
+      <c r="F32" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D39" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E39" s="2">
-        <f>SUM(E2:E30)</f>
-        <v>3255</v>
+        <f>SUM(E2:E32)</f>
+        <v>3540</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
@@ -1273,7 +1328,7 @@
       </c>
       <c r="E40" s="2">
         <f>E39 / 60</f>
-        <v>54.25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Scheduling, Gantt Chart and Work Breakdown Structure
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Log Book.xlsx
+++ b/Documentation/Complete Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="278" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C0E80C7-A9A8-4277-8727-7C6462E9DFEC}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2F4AAD8-C267-4E2B-9439-84FF9CBFE8ED}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>Research Methdologies Suitable for Individual Projects, Document Waterfall, TDD, KanBan, and Justify Chosen Methodologies</t>
+  </si>
+  <si>
+    <t>ProjectLibre</t>
+  </si>
+  <si>
+    <t>Tutorials on How to Use ProjectLibre Software</t>
+  </si>
+  <si>
+    <t>Create Work Breakdown Structure and Gantt Chart with Project Libre</t>
   </si>
 </sst>
 </file>
@@ -660,7 +669,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1322,47 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33">
+        <v>20</v>
+      </c>
+      <c r="F33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1322,7 +1371,7 @@
         <v>3540</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1331,7 +1380,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Literature Review: Music Notations, Terminology, Keyboard Ghosting
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Log Book.xlsx
+++ b/Documentation/Complete Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="289" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2F4AAD8-C267-4E2B-9439-84FF9CBFE8ED}"/>
+  <xr:revisionPtr revIDLastSave="297" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE943372-207E-4070-916C-3866F8B5E145}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>Create Work Breakdown Structure and Gantt Chart with Project Libre</t>
+  </si>
+  <si>
+    <t>Literature Review</t>
+  </si>
+  <si>
+    <t>Music Notations, Terminology, Keyboard Ghosting and Diagrams</t>
   </si>
 </sst>
 </file>
@@ -669,7 +675,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,13 +1368,33 @@
         <v>82</v>
       </c>
     </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35">
+        <v>180</v>
+      </c>
+      <c r="F35" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D39" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E39" s="2">
-        <f>SUM(E2:E32)</f>
-        <v>3540</v>
+        <f>SUM(E2:E35)</f>
+        <v>3840</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1377,7 +1403,7 @@
       </c>
       <c r="E40" s="2">
         <f>E39 / 60</f>
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Logarithmic and Linear Ladders
</commit_message>
<xml_diff>
--- a/Documentation/Complete Project Log Book.xlsx
+++ b/Documentation/Complete Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3FEAF4E-AB2F-46C2-ADBB-9494CD76EEA3}"/>
+  <xr:revisionPtr revIDLastSave="324" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C012BE7-CC02-4F7F-BBCB-554941A759DF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -309,6 +309,18 @@
   </si>
   <si>
     <t>Research on Logarithmic Laddre Solutions</t>
+  </si>
+  <si>
+    <t>Research on Linear Laddre Solutions, Algorithms and Diagrams</t>
+  </si>
+  <si>
+    <t>21.10.2022</t>
+  </si>
+  <si>
+    <t>Linear Ladder</t>
+  </si>
+  <si>
+    <t>Research on Linear Laddre Solutions, Algorithms and Diagrams and R2R Ladders</t>
   </si>
 </sst>
 </file>
@@ -690,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,35 +1458,75 @@
         <v>90</v>
       </c>
     </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38">
+        <v>210</v>
+      </c>
+      <c r="F38" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D39" s="2" t="s">
+      <c r="A39" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39">
+        <v>190</v>
+      </c>
+      <c r="F39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="2">
-        <f>SUM(E2:E37)</f>
-        <v>4005</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D40" s="2" t="s">
+      <c r="E49" s="2">
+        <f>SUM(E2:E39)</f>
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="2">
-        <f>E39 / 60</f>
-        <v>66.75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="E50" s="2">
+        <f>E49 / 60</f>
+        <v>73.416666666666671</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>37</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D51" t="s">
         <v>40</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E51" t="s">
         <v>36</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F51" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>